<commit_message>
shop_server-2 #2 swagger UI 추가 - swaggerUI 추가
</commit_message>
<xml_diff>
--- a/구매사이트_ERD.xlsx
+++ b/구매사이트_ERD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\IdeaProjects\workSpace\shop_server\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="147">
   <si>
     <t>테이블명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -362,18 +362,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>use_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>use_pwd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>use_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>user_phone</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -619,6 +607,14 @@
   </si>
   <si>
     <t>NonuserOrder_detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_pwd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1099,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1836,10 +1832,10 @@
         <v>81</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>24</v>
@@ -1857,10 +1853,10 @@
         <v>81</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>84</v>
+        <v>145</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>25</v>
@@ -1878,13 +1874,13 @@
         <v>81</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>29</v>
@@ -1899,13 +1895,13 @@
         <v>81</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>29</v>
@@ -1920,10 +1916,10 @@
         <v>81</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>25</v>
@@ -1941,13 +1937,13 @@
         <v>81</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>29</v>
@@ -1962,13 +1958,13 @@
         <v>81</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>29</v>
@@ -1983,10 +1979,10 @@
         <v>81</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>72</v>
@@ -2004,10 +2000,10 @@
         <v>81</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>26</v>
@@ -2025,13 +2021,13 @@
         <v>81</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>29</v>
@@ -2046,10 +2042,10 @@
         <v>81</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F44" s="11" t="s">
         <v>28</v>
@@ -2066,13 +2062,13 @@
         <v>82</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>26</v>
@@ -2089,13 +2085,13 @@
         <v>82</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>24</v>
@@ -2110,13 +2106,13 @@
         <v>82</v>
       </c>
       <c r="C47" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>110</v>
-      </c>
       <c r="E47" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>28</v>
@@ -2131,16 +2127,16 @@
         <v>82</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>29</v>
@@ -2152,13 +2148,13 @@
         <v>82</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>25</v>
@@ -2173,13 +2169,13 @@
         <v>82</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>25</v>
@@ -2194,16 +2190,16 @@
         <v>82</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>29</v>
@@ -2215,16 +2211,16 @@
         <v>82</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G52" s="11" t="s">
         <v>29</v>
@@ -2235,16 +2231,16 @@
         <v>30</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>26</v>
@@ -2258,16 +2254,16 @@
         <v>38</v>
       </c>
       <c r="B54" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>126</v>
-      </c>
       <c r="E54" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>26</v>
@@ -2279,16 +2275,16 @@
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C55" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="E55" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>71</v>
@@ -2300,16 +2296,16 @@
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>71</v>
@@ -2321,16 +2317,16 @@
     <row r="57" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="11"/>
       <c r="B57" s="12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>25</v>
@@ -2344,16 +2340,16 @@
         <v>30</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>26</v>
@@ -2367,16 +2363,16 @@
         <v>38</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F59" s="8" t="s">
         <v>26</v>
@@ -2390,10 +2386,10 @@
         <v>38</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>8</v>
@@ -2411,10 +2407,10 @@
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>77</v>
@@ -2432,10 +2428,10 @@
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>11</v>
@@ -2453,19 +2449,19 @@
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>29</v>
@@ -2474,16 +2470,16 @@
     <row r="64" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="11"/>
       <c r="B64" s="12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C64" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D64" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D64" s="13" t="s">
-        <v>136</v>
-      </c>
       <c r="E64" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F64" s="11" t="s">
         <v>72</v>
@@ -2497,16 +2493,16 @@
         <v>30</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>26</v>
@@ -2518,16 +2514,16 @@
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>28</v>
@@ -2539,19 +2535,19 @@
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>29</v>
@@ -2560,16 +2556,16 @@
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>143</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>25</v>
@@ -2581,16 +2577,16 @@
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C69" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>25</v>
@@ -2602,19 +2598,19 @@
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>29</v>
@@ -2623,19 +2619,19 @@
     <row r="71" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="11"/>
       <c r="B71" s="12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E71" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G71" s="11" t="s">
         <v>29</v>
@@ -2646,16 +2642,16 @@
         <v>30</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>26</v>
@@ -2669,16 +2665,16 @@
         <v>38</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>26</v>
@@ -2690,16 +2686,16 @@
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>71</v>
@@ -2711,16 +2707,16 @@
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>71</v>
@@ -2732,16 +2728,16 @@
     <row r="76" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="11"/>
       <c r="B76" s="12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>25</v>
@@ -2755,16 +2751,16 @@
         <v>30</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F77" s="8" t="s">
         <v>26</v>
@@ -2778,16 +2774,16 @@
         <v>38</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>26</v>
@@ -2801,10 +2797,10 @@
         <v>38</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>8</v>
@@ -2822,10 +2818,10 @@
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>77</v>
@@ -2843,10 +2839,10 @@
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>11</v>
@@ -2864,19 +2860,19 @@
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
       <c r="B82" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>29</v>
@@ -2885,16 +2881,16 @@
     <row r="83" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="11"/>
       <c r="B83" s="12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F83" s="11" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
#4 QueryDSL * QueryDSL 적용 - select 쿼리만 수행 * Dao 삭제
</commit_message>
<xml_diff>
--- a/구매사이트_ERD.xlsx
+++ b/구매사이트_ERD.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="145">
   <si>
     <t>테이블명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,10 +58,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Product</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>product_number</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -154,10 +150,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Product_category</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>category_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -514,18 +506,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UserOrder_refund</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>refund_number</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>order_derail_number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>refund_reason</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -550,10 +534,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UserOrder_detail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>order_detail_number</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -582,10 +562,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Nonuser_Order</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>배송지주소1(우편번호)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -598,23 +574,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NonuserOrder_refund</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>refund_email</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NonuserOrder_detail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>user_pwd</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>user_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nonuser_order</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product_category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_order_refund</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_order_detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nonuser_order_detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nonuser_order_refund</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -670,7 +662,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -721,13 +713,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -770,6 +786,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -792,15 +817,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>112532</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>65761</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>426857</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>180061</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -817,7 +842,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="371475" y="295275"/>
+          <a:off x="0" y="1247775"/>
           <a:ext cx="14142857" cy="7314286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1093,21 +1118,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G147"/>
+  <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34:D44"/>
+    <sheetView tabSelected="1" topLeftCell="C55" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
+    <col min="1" max="1" width="15.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.125" customWidth="1"/>
-    <col min="5" max="5" width="27.25" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1122,59 +1147,59 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>16</v>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1183,19 +1208,19 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1204,19 +1229,19 @@
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1225,19 +1250,19 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1246,19 +1271,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1267,19 +1292,19 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>29</v>
+      <c r="G8" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1288,42 +1313,42 @@
         <v>6</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>31</v>
+        <v>140</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>34</v>
+        <v>8</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1332,19 +1357,19 @@
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>31</v>
+        <v>140</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1353,65 +1378,65 @@
         <v>6</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>36</v>
+      <c r="E12" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>48</v>
+      <c r="E13" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1420,19 +1445,19 @@
         <v>6</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>49</v>
+        <v>40</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1441,19 +1466,19 @@
         <v>6</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1462,19 +1487,19 @@
         <v>6</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>29</v>
+      <c r="G17" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1483,19 +1508,19 @@
         <v>6</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1504,19 +1529,19 @@
         <v>6</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1525,65 +1550,65 @@
         <v>6</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>29</v>
+        <v>53</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1592,19 +1617,19 @@
         <v>6</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1613,19 +1638,19 @@
         <v>6</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>67</v>
+        <v>55</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1634,19 +1659,19 @@
         <v>6</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1655,19 +1680,19 @@
         <v>6</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1676,19 +1701,19 @@
         <v>6</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1697,19 +1722,19 @@
         <v>6</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>29</v>
+      <c r="G28" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1718,1185 +1743,1185 @@
         <v>6</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>70</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>29</v>
+      <c r="E30" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C31" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="15"/>
+      <c r="B32" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E32" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="13" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11"/>
       <c r="B33" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>80</v>
+        <v>75</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>91</v>
+        <v>104</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>29</v>
+        <v>137</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>29</v>
+        <v>138</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C37" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>29</v>
+      <c r="E37" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>29</v>
+      <c r="E38" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>29</v>
+        <v>83</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>29</v>
+        <v>84</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>29</v>
+        <v>85</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>98</v>
+        <v>86</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>29</v>
+        <v>87</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11"/>
       <c r="B44" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>100</v>
+        <v>88</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="F44" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G44" s="11" t="s">
-        <v>29</v>
+      <c r="G44" s="13" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>29</v>
+        <v>103</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C46" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>91</v>
+      <c r="E46" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>114</v>
+        <v>105</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>29</v>
+      <c r="G47" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>115</v>
+        <v>106</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>116</v>
+        <v>107</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>117</v>
+        <v>108</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>118</v>
+        <v>109</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11"/>
       <c r="B52" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>119</v>
+        <v>110</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="D53" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G53" s="10" t="s">
         <v>122</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="D54" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C55" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="D55" s="5" t="s">
+      <c r="E55" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C56" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="E56" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="11"/>
       <c r="B57" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="E57" s="13" t="s">
-        <v>94</v>
+        <v>82</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G57" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>29</v>
+        <v>126</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>29</v>
+        <v>103</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>29</v>
+        <v>7</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>29</v>
+        <v>75</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="11"/>
       <c r="B64" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C64" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G64" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="D64" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="E64" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F64" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G64" s="11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>113</v>
+        <v>103</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G65" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>114</v>
+        <v>105</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G66" s="3" t="s">
-        <v>29</v>
+      <c r="G66" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>139</v>
+        <v>106</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>140</v>
+        <v>107</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>141</v>
+        <v>108</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>118</v>
+        <v>109</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="11"/>
       <c r="B71" s="12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E71" s="13" t="s">
-        <v>119</v>
+        <v>110</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="G71" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G71" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D72" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G72" s="10" t="s">
         <v>122</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="F72" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G72" s="8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>142</v>
+        <v>131</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>142</v>
+        <v>131</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="D74" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G74" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>142</v>
+        <v>131</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="D75" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G75" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="11"/>
       <c r="B76" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D76" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C76" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D76" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="E76" s="13" t="s">
-        <v>94</v>
+      <c r="E76" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="G76" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F77" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>29</v>
+        <v>126</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>113</v>
+        <v>103</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
       <c r="B82" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="11"/>
       <c r="B83" s="12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="E83" s="13" t="s">
-        <v>135</v>
+        <v>128</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G83" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G83" s="13" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -2904,576 +2929,576 @@
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
       <c r="D84" s="10"/>
-      <c r="E84" s="10"/>
+      <c r="E84" s="8"/>
       <c r="F84" s="8"/>
-      <c r="G84" s="8"/>
+      <c r="G84" s="10"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
+      <c r="E85" s="3"/>
       <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
+      <c r="G85" s="5"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
+      <c r="E86" s="3"/>
       <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
+      <c r="G86" s="5"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
+      <c r="E87" s="3"/>
       <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
+      <c r="G87" s="5"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
+      <c r="E88" s="3"/>
       <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
+      <c r="G88" s="5"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
+      <c r="E89" s="3"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
+      <c r="G89" s="5"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
+      <c r="E90" s="3"/>
       <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
+      <c r="G90" s="5"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
+      <c r="E91" s="3"/>
       <c r="F91" s="3"/>
-      <c r="G91" s="3"/>
+      <c r="G91" s="5"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
+      <c r="E92" s="3"/>
       <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
+      <c r="G92" s="5"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
+      <c r="E93" s="3"/>
       <c r="F93" s="3"/>
-      <c r="G93" s="3"/>
+      <c r="G93" s="5"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
+      <c r="E94" s="3"/>
       <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
+      <c r="G94" s="5"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
+      <c r="E95" s="3"/>
       <c r="F95" s="3"/>
-      <c r="G95" s="3"/>
+      <c r="G95" s="5"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
+      <c r="E96" s="3"/>
       <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
+      <c r="G96" s="5"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
+      <c r="E97" s="3"/>
       <c r="F97" s="3"/>
-      <c r="G97" s="3"/>
+      <c r="G97" s="5"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
+      <c r="E98" s="3"/>
       <c r="F98" s="3"/>
-      <c r="G98" s="3"/>
+      <c r="G98" s="5"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
+      <c r="E99" s="3"/>
       <c r="F99" s="3"/>
-      <c r="G99" s="3"/>
+      <c r="G99" s="5"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
+      <c r="E100" s="3"/>
       <c r="F100" s="3"/>
-      <c r="G100" s="3"/>
+      <c r="G100" s="5"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
+      <c r="E101" s="3"/>
       <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
+      <c r="G101" s="5"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
+      <c r="E102" s="3"/>
       <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
+      <c r="G102" s="5"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
+      <c r="E103" s="3"/>
       <c r="F103" s="3"/>
-      <c r="G103" s="3"/>
+      <c r="G103" s="5"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
+      <c r="E104" s="3"/>
       <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
+      <c r="G104" s="5"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
+      <c r="E105" s="3"/>
       <c r="F105" s="3"/>
-      <c r="G105" s="3"/>
+      <c r="G105" s="5"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="3"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
+      <c r="E106" s="3"/>
       <c r="F106" s="3"/>
-      <c r="G106" s="3"/>
+      <c r="G106" s="5"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
+      <c r="E107" s="3"/>
       <c r="F107" s="3"/>
-      <c r="G107" s="3"/>
+      <c r="G107" s="5"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="5"/>
-      <c r="E108" s="5"/>
+      <c r="E108" s="3"/>
       <c r="F108" s="3"/>
-      <c r="G108" s="3"/>
+      <c r="G108" s="5"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="3"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="5"/>
-      <c r="E109" s="5"/>
+      <c r="E109" s="3"/>
       <c r="F109" s="3"/>
-      <c r="G109" s="3"/>
+      <c r="G109" s="5"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="3"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="5"/>
-      <c r="E110" s="5"/>
+      <c r="E110" s="3"/>
       <c r="F110" s="3"/>
-      <c r="G110" s="3"/>
+      <c r="G110" s="5"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="3"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
       <c r="D111" s="5"/>
-      <c r="E111" s="5"/>
+      <c r="E111" s="3"/>
       <c r="F111" s="3"/>
-      <c r="G111" s="3"/>
+      <c r="G111" s="5"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
+      <c r="E112" s="3"/>
       <c r="F112" s="3"/>
-      <c r="G112" s="3"/>
+      <c r="G112" s="5"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="3"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
+      <c r="E113" s="3"/>
       <c r="F113" s="3"/>
-      <c r="G113" s="3"/>
+      <c r="G113" s="5"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="3"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="5"/>
-      <c r="E114" s="5"/>
+      <c r="E114" s="3"/>
       <c r="F114" s="3"/>
-      <c r="G114" s="3"/>
+      <c r="G114" s="5"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="5"/>
-      <c r="E115" s="5"/>
+      <c r="E115" s="3"/>
       <c r="F115" s="3"/>
-      <c r="G115" s="3"/>
+      <c r="G115" s="5"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="5"/>
-      <c r="E116" s="5"/>
+      <c r="E116" s="3"/>
       <c r="F116" s="3"/>
-      <c r="G116" s="3"/>
+      <c r="G116" s="5"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
       <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
+      <c r="E117" s="3"/>
       <c r="F117" s="3"/>
-      <c r="G117" s="3"/>
+      <c r="G117" s="5"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="3"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
+      <c r="E118" s="3"/>
       <c r="F118" s="3"/>
-      <c r="G118" s="3"/>
+      <c r="G118" s="5"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
+      <c r="E119" s="3"/>
       <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
+      <c r="G119" s="5"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
       <c r="D120" s="5"/>
-      <c r="E120" s="5"/>
+      <c r="E120" s="3"/>
       <c r="F120" s="3"/>
-      <c r="G120" s="3"/>
+      <c r="G120" s="5"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="3"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
       <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
+      <c r="E121" s="3"/>
       <c r="F121" s="3"/>
-      <c r="G121" s="3"/>
+      <c r="G121" s="5"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="3"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
       <c r="D122" s="5"/>
-      <c r="E122" s="5"/>
+      <c r="E122" s="3"/>
       <c r="F122" s="3"/>
-      <c r="G122" s="3"/>
+      <c r="G122" s="5"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="3"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
       <c r="D123" s="5"/>
-      <c r="E123" s="5"/>
+      <c r="E123" s="3"/>
       <c r="F123" s="3"/>
-      <c r="G123" s="3"/>
+      <c r="G123" s="5"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="3"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
       <c r="D124" s="5"/>
-      <c r="E124" s="5"/>
+      <c r="E124" s="3"/>
       <c r="F124" s="3"/>
-      <c r="G124" s="3"/>
+      <c r="G124" s="5"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="5"/>
-      <c r="E125" s="5"/>
+      <c r="E125" s="3"/>
       <c r="F125" s="3"/>
-      <c r="G125" s="3"/>
+      <c r="G125" s="5"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="3"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="5"/>
-      <c r="E126" s="5"/>
+      <c r="E126" s="3"/>
       <c r="F126" s="3"/>
-      <c r="G126" s="3"/>
+      <c r="G126" s="5"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="5"/>
-      <c r="E127" s="5"/>
+      <c r="E127" s="3"/>
       <c r="F127" s="3"/>
-      <c r="G127" s="3"/>
+      <c r="G127" s="5"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="5"/>
-      <c r="E128" s="5"/>
+      <c r="E128" s="3"/>
       <c r="F128" s="3"/>
-      <c r="G128" s="3"/>
+      <c r="G128" s="5"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
       <c r="D129" s="5"/>
-      <c r="E129" s="5"/>
+      <c r="E129" s="3"/>
       <c r="F129" s="3"/>
-      <c r="G129" s="3"/>
+      <c r="G129" s="5"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
       <c r="D130" s="5"/>
-      <c r="E130" s="5"/>
+      <c r="E130" s="3"/>
       <c r="F130" s="3"/>
-      <c r="G130" s="3"/>
+      <c r="G130" s="5"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="5"/>
-      <c r="E131" s="5"/>
+      <c r="E131" s="3"/>
       <c r="F131" s="3"/>
-      <c r="G131" s="3"/>
+      <c r="G131" s="5"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
       <c r="D132" s="5"/>
-      <c r="E132" s="5"/>
+      <c r="E132" s="3"/>
       <c r="F132" s="3"/>
-      <c r="G132" s="3"/>
+      <c r="G132" s="5"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
       <c r="D133" s="5"/>
-      <c r="E133" s="5"/>
+      <c r="E133" s="3"/>
       <c r="F133" s="3"/>
-      <c r="G133" s="3"/>
+      <c r="G133" s="5"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
       <c r="D134" s="5"/>
-      <c r="E134" s="5"/>
+      <c r="E134" s="3"/>
       <c r="F134" s="3"/>
-      <c r="G134" s="3"/>
+      <c r="G134" s="5"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
       <c r="D135" s="5"/>
-      <c r="E135" s="5"/>
+      <c r="E135" s="3"/>
       <c r="F135" s="3"/>
-      <c r="G135" s="3"/>
+      <c r="G135" s="5"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
       <c r="D136" s="5"/>
-      <c r="E136" s="5"/>
+      <c r="E136" s="3"/>
       <c r="F136" s="3"/>
-      <c r="G136" s="3"/>
+      <c r="G136" s="5"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
       <c r="D137" s="5"/>
-      <c r="E137" s="5"/>
+      <c r="E137" s="3"/>
       <c r="F137" s="3"/>
-      <c r="G137" s="3"/>
+      <c r="G137" s="5"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="3"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="5"/>
-      <c r="E138" s="5"/>
+      <c r="E138" s="3"/>
       <c r="F138" s="3"/>
-      <c r="G138" s="3"/>
+      <c r="G138" s="5"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="3"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="5"/>
-      <c r="E139" s="5"/>
+      <c r="E139" s="3"/>
       <c r="F139" s="3"/>
-      <c r="G139" s="3"/>
+      <c r="G139" s="5"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="3"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
       <c r="D140" s="5"/>
-      <c r="E140" s="5"/>
+      <c r="E140" s="3"/>
       <c r="F140" s="3"/>
-      <c r="G140" s="3"/>
+      <c r="G140" s="5"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="3"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="D141" s="5"/>
-      <c r="E141" s="5"/>
+      <c r="E141" s="3"/>
       <c r="F141" s="3"/>
-      <c r="G141" s="3"/>
+      <c r="G141" s="5"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="3"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="5"/>
-      <c r="E142" s="5"/>
+      <c r="E142" s="3"/>
       <c r="F142" s="3"/>
-      <c r="G142" s="3"/>
+      <c r="G142" s="5"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="3"/>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
       <c r="D143" s="5"/>
-      <c r="E143" s="5"/>
+      <c r="E143" s="3"/>
       <c r="F143" s="3"/>
-      <c r="G143" s="3"/>
+      <c r="G143" s="5"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="3"/>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
       <c r="D144" s="5"/>
-      <c r="E144" s="5"/>
+      <c r="E144" s="3"/>
       <c r="F144" s="3"/>
-      <c r="G144" s="3"/>
+      <c r="G144" s="5"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="3"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
       <c r="D145" s="5"/>
-      <c r="E145" s="5"/>
+      <c r="E145" s="3"/>
       <c r="F145" s="3"/>
-      <c r="G145" s="3"/>
+      <c r="G145" s="5"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="3"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
       <c r="D146" s="5"/>
-      <c r="E146" s="5"/>
+      <c r="E146" s="3"/>
       <c r="F146" s="3"/>
-      <c r="G146" s="3"/>
+      <c r="G146" s="5"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="3"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
       <c r="D147" s="5"/>
-      <c r="E147" s="5"/>
+      <c r="E147" s="3"/>
       <c r="F147" s="3"/>
-      <c r="G147" s="3"/>
+      <c r="G147" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1"/>
@@ -3487,7 +3512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>